<commit_message>
Changed SQL files and adjust API files
</commit_message>
<xml_diff>
--- a/Project1/ERD-Tables/F1-ERD.xlsx
+++ b/Project1/ERD-Tables/F1-ERD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51fc7d7ba1648333/Semester 2/Web Development Fundamentals/Project1/ERD-Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalProj\PProj\Project1\ERD-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="622" documentId="8_{A094AFAC-0568-443C-852D-1C815C90C3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9ECC02-0E50-4958-8D3B-D1077A4A6122}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A507B17-83B4-4190-A321-5D3F00CDF888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FACCED06-140A-4EE2-91B2-4736CEB3626B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{FACCED06-140A-4EE2-91B2-4736CEB3626B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="203">
   <si>
     <t>F1 Database</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Primary Key</t>
   </si>
   <si>
-    <t>Foreign Key</t>
-  </si>
-  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>Format</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>PK/FK</t>
   </si>
   <si>
@@ -608,43 +602,49 @@
     <t>number of turns on the track</t>
   </si>
   <si>
-    <t>favouriteTeam</t>
-  </si>
-  <si>
     <t>favouriteDriver</t>
   </si>
   <si>
-    <t>SeasonID</t>
-  </si>
-  <si>
-    <t>All Time</t>
-  </si>
-  <si>
-    <t>AllTimeID</t>
-  </si>
-  <si>
-    <t>mostWins</t>
-  </si>
-  <si>
-    <t>mostPodiums</t>
-  </si>
-  <si>
-    <t>mostPoles</t>
-  </si>
-  <si>
-    <t>mostFastestLaps</t>
-  </si>
-  <si>
-    <t>mostConstructorWins</t>
-  </si>
-  <si>
-    <t>mostDriversChampionships</t>
-  </si>
-  <si>
-    <t>mostConstructorChampionships</t>
-  </si>
-  <si>
-    <t>constructorChampionships</t>
+    <t>favouriteConstructor</t>
+  </si>
+  <si>
+    <t>fastest</t>
+  </si>
+  <si>
+    <t>Races</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Constructors</t>
+  </si>
+  <si>
+    <t>Drivers</t>
+  </si>
+  <si>
+    <t>tireCompound</t>
+  </si>
+  <si>
+    <t>seasonsWithConstructor</t>
+  </si>
+  <si>
+    <t>seasonID</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>constructorTitles</t>
+  </si>
+  <si>
+    <t>startYear</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -756,17 +756,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -795,36 +784,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
@@ -833,19 +792,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -865,19 +811,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
       <right style="thin">
@@ -888,19 +821,6 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -939,19 +859,6 @@
       <bottom style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1014,17 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
@@ -1036,13 +932,58 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1050,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1067,16 +1008,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,58 +1029,55 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,27 +1089,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1195,10 +1107,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1518,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE95D0D-B825-401D-9EF3-14CD69F00698}">
-  <dimension ref="A1:L133"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,14 +1439,13 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="81.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="31" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1547,10 +1454,11 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1559,22 +1467,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1584,9 +1489,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1596,726 +1500,626 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>7</v>
+        <v>194</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="I5" s="7"/>
       <c r="J5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="L5" s="42"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="H6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="L6" s="43"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I7" s="7"/>
       <c r="J7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="L7" s="44"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I8" s="7"/>
       <c r="J8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L8" s="44"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L9" s="44"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="I10" s="7"/>
       <c r="J10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L10" s="46"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>50</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>76</v>
+        <v>29</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="L11" s="46"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>77</v>
+        <v>46</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="8"/>
+      <c r="B17" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="29"/>
       <c r="D17" s="1"/>
       <c r="E17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="26"/>
+        <v>70</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="19"/>
+      <c r="E20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="30"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="40"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="29"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F25" s="20"/>
-      <c r="G25" s="28"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="28"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="28"/>
+      <c r="F24" s="26"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="E26" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="F26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="G26" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="H26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="16" t="s">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="H27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D28" s="1">
         <v>50</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D29" s="1">
         <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1">
         <v>50</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" s="1">
         <v>255</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="1">
         <v>100</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D34" s="1">
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2323,9 +2127,8 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2333,9 +2136,8 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2343,9 +2145,8 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2353,11 +2154,10 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2365,185 +2165,175 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D43" s="1">
         <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="1">
         <v>50</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="1">
         <v>30</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D47" s="1">
         <v>100</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
-        <v>52</v>
+      <c r="H47" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D48" s="1">
         <v>10</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D49" s="1">
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
-        <v>20</v>
+      <c r="H49" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2551,109 +2341,103 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D53" s="1">
         <v>100</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D54" s="1">
         <v>100</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D55" s="1">
         <v>50</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D56" s="1">
         <v>50</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2661,275 +2445,260 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D59" s="1">
         <v>100</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D61" s="1">
         <v>100</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D62" s="1">
         <v>50</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H62" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D63" s="1">
         <v>30</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H63" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D64" s="1">
         <v>50</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H65" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H66" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D67" s="1">
         <v>20</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H67" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D68" s="1">
         <v>50</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1" t="s">
+      <c r="H68" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H69" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H70" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H71" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2937,87 +2706,82 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H73" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D74" s="1">
         <v>50</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H74" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D75" s="1">
         <v>100</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="7" t="s">
-        <v>40</v>
+      <c r="H75" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H76" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3025,283 +2789,267 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H78" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H79" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="8" t="s">
-        <v>48</v>
+      <c r="H80" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="8" t="s">
-        <v>49</v>
+      <c r="H81" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="8" t="s">
-        <v>62</v>
+      <c r="H82" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="8" t="s">
-        <v>61</v>
+      <c r="H83" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H84" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
-        <v>59</v>
+      <c r="H85" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="8" t="s">
-        <v>68</v>
+      <c r="H86" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="8" t="s">
-        <v>57</v>
+      <c r="H87" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="8" t="s">
-        <v>69</v>
+      <c r="H88" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="8" t="s">
-        <v>67</v>
+      <c r="H89" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D90" s="1">
         <v>50</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="7" t="s">
-        <v>24</v>
+      <c r="H90" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="7" t="s">
-        <v>17</v>
+      <c r="H91" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H92" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -3309,251 +3057,237 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H94" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D95" s="1">
         <v>100</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H95" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D96" s="1">
         <v>50</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H96" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D97" s="1">
         <v>50</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H97" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="8" t="s">
-        <v>32</v>
+      <c r="H98" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="8" t="s">
-        <v>33</v>
+      <c r="H99" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B101" s="8" t="s">
-        <v>74</v>
+      <c r="H100" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="8" t="s">
-        <v>76</v>
+      <c r="H101" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="8" t="s">
-        <v>77</v>
+      <c r="H102" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B104" s="8" t="s">
-        <v>78</v>
+      <c r="H103" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B105" s="7" t="s">
-        <v>17</v>
+      <c r="H104" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="7" t="s">
-        <v>20</v>
+      <c r="H105" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H106" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -3561,173 +3295,163 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-    </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H108" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H109" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H110" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H111" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H112" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H113" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-      <c r="I114" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="7" t="s">
-        <v>17</v>
+      <c r="H114" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="7" t="s">
-        <v>20</v>
+      <c r="H115" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H116" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -3735,145 +3459,137 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
-      <c r="I117" s="1"/>
-    </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H118" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D119" s="1">
         <v>255</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H119" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H120" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D121" s="1">
         <v>100</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-      <c r="I121" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H121" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H122" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D123" s="1">
         <v>50</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-      <c r="I123" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H123" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D124" s="1">
         <v>255</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-      <c r="I124" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H124" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -3881,123 +3597,120 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
-    </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H126" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D127" s="1">
         <v>100</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
-      <c r="H127" s="1"/>
-      <c r="I127" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H127" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D128" s="1">
         <v>100</v>
       </c>
-      <c r="I128" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H128" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D129" s="1">
         <v>50</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D130" s="1">
         <v>50</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I130" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H132" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B131" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="3"/>
     </row>
   </sheetData>

</xml_diff>